<commit_message>
Added encoding for links in Excel, but spaces are still not supported, just don't throw exceptions.
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\Beton\Beton\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\Beton\Beton\src\main\resources\dataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>Item</t>
   </si>
@@ -714,10 +714,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,20 +775,9 @@
         <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added testng_IOS.xml and community signin_IOS
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData.xlsx
@@ -5,20 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\Beton\Beton\src\main\resources\dataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajp.NEXPERIENCE\Desktop\FrameworkTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080"/>
   </bookViews>
   <sheets>
-    <sheet name="devices (2)" sheetId="19" r:id="rId1"/>
+    <sheet name="devices" sheetId="11" r:id="rId1"/>
     <sheet name="signIn" sheetId="18" r:id="rId2"/>
-    <sheet name="devices" sheetId="11" r:id="rId3"/>
-    <sheet name="items" sheetId="1" r:id="rId4"/>
-    <sheet name="addresses" sheetId="7" r:id="rId5"/>
+    <sheet name="items" sheetId="1" r:id="rId3"/>
+    <sheet name="addresses" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Item</t>
   </si>
@@ -126,21 +125,12 @@
     <t>iPhone-6</t>
   </si>
   <si>
-    <t>mobileOS</t>
-  </si>
-  <si>
     <t>$6.26</t>
   </si>
   <si>
     <t>$59.00</t>
   </si>
   <si>
-    <t>Avner</t>
-  </si>
-  <si>
-    <t>Galaxy S5 SM-G900A</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -180,10 +170,7 @@
     <t>Brian</t>
   </si>
   <si>
-    <t>ShirNate</t>
-  </si>
-  <si>
-    <t>Raj</t>
+    <t>SAFARI</t>
   </si>
 </sst>
 </file>
@@ -527,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="A6:J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,54 +575,10 @@
         <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -649,7 +592,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,46 +604,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -713,81 +656,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -821,7 +689,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -843,7 +711,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -852,7 +720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Excel auto column size in @AfterClass method.
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajp\git\Beton\Beton\src\main\resources\dataSheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11505" windowHeight="6315"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="11" r:id="rId1"/>
@@ -17,7 +12,8 @@
     <sheet name="items" sheetId="1" r:id="rId3"/>
     <sheet name="addresses" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:H19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -703,7 +699,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>

</xml_diff>

<commit_message>
Created new package androidCommunityPOM_Appium to use the Appium AndroidDriver including a modified PerfectoAppiumUtils class. Added BasicTest_Android that takes an Appium AndroidDriver to com.perfectomobile.test. Modified CommunitySignIn_Android test case to handle the Appium AndroidDriver.
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\Beton\Beton\src\main\resources\dataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PerfectoBC\git\Beton\Beton\src\main\resources\dataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Item</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Raj</t>
+  </si>
+  <si>
+    <t>Galaxy S5</t>
   </si>
 </sst>
 </file>
@@ -714,10 +717,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,12 +775,23 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J3" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>